<commit_message>
Deploy updated output folder for publication
</commit_message>
<xml_diff>
--- a/CodeSystem-NGStockReportCS.xlsx
+++ b/CodeSystem-NGStockReportCS.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.4.0</t>
+    <t>0.5.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-04T18:56:28+01:00</t>
+    <t>2025-07-04T19:33:02+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>